<commit_message>
Added test data for RAD Existing Liability Test Cases
</commit_message>
<xml_diff>
--- a/VLinkCCTestData.xlsx
+++ b/VLinkCCTestData.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8385" uniqueCount="838">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8841" uniqueCount="952">
   <si>
     <t>Notes</t>
   </si>
@@ -2549,6 +2549,348 @@
   </si>
   <si>
     <t>Sun Aug 22 17:03:41 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:20:26 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:21:34 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:22:35 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:23:37 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:24:37 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:25:38 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:26:39 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:27:40 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:28:40 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:29:42 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:30:43 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:31:43 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:32:45 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:33:45 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:34:45 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:35:47 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:36:47 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:37:48 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:38:48 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:39:49 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:40:50 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:41:51 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:42:51 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:43:52 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:44:55 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:45:55 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:46:56 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:47:58 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:48:59 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:50:02 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:51:04 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:52:06 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:53:06 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:54:09 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:55:09 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:56:10 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:57:13 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:58:17 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 13:59:18 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:00:22 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:01:26 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:02:27 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:03:30 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:04:31 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:05:34 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:06:36 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:07:37 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:08:40 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:09:43 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:10:43 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:11:45 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:12:46 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:13:48 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:14:48 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:15:50 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:16:52 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:17:54 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:18:55 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:19:58 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:20:59 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:22:01 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:23:02 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:24:04 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:25:06 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:26:07 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:27:09 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:28:12 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:29:13 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:30:16 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:31:18 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:32:20 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:33:22 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:34:23 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:35:24 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:36:25 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:37:26 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:38:27 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:39:28 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:40:30 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:41:31 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:42:33 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:43:34 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:44:36 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:45:37 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:46:39 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:47:41 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:48:43 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:49:45 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:50:47 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:51:49 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:52:50 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:53:52 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:54:54 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:55:56 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:56:58 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:58:00 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 14:59:02 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:00:03 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:01:04 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:02:05 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:03:08 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:04:10 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:05:12 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:06:12 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:07:12 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:08:13 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:09:14 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:10:15 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:11:14 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:12:15 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:13:17 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:14:19 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:15:19 EDT 2021</t>
+  </si>
+  <si>
+    <t>Sun Oct 31 15:16:21 EDT 2021</t>
   </si>
 </sst>
 </file>
@@ -3146,7 +3488,7 @@
         <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>724</v>
+        <v>838</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>43</v>
@@ -3260,7 +3602,7 @@
         <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>725</v>
+        <v>839</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>43</v>
@@ -3321,7 +3663,7 @@
         <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>726</v>
+        <v>840</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>43</v>
@@ -3382,7 +3724,7 @@
         <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>727</v>
+        <v>841</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>43</v>
@@ -3496,7 +3838,7 @@
         <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>728</v>
+        <v>842</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>43</v>
@@ -3557,7 +3899,7 @@
         <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>729</v>
+        <v>843</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>43</v>
@@ -3618,7 +3960,7 @@
         <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>730</v>
+        <v>844</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>43</v>
@@ -3732,7 +4074,7 @@
         <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>731</v>
+        <v>845</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>43</v>
@@ -3793,7 +4135,7 @@
         <v>149</v>
       </c>
       <c r="B10" t="s">
-        <v>732</v>
+        <v>846</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>43</v>
@@ -3854,7 +4196,7 @@
         <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>733</v>
+        <v>847</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>43</v>
@@ -3968,7 +4310,7 @@
         <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>734</v>
+        <v>848</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>43</v>
@@ -4029,7 +4371,7 @@
         <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>735</v>
+        <v>849</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>43</v>
@@ -4090,7 +4432,7 @@
         <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>736</v>
+        <v>850</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>43</v>
@@ -4204,7 +4546,7 @@
         <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>737</v>
+        <v>851</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>43</v>
@@ -4265,7 +4607,7 @@
         <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>738</v>
+        <v>852</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>43</v>
@@ -4326,7 +4668,7 @@
         <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>739</v>
+        <v>853</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>43</v>
@@ -4440,7 +4782,7 @@
         <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>740</v>
+        <v>854</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>43</v>
@@ -4501,7 +4843,7 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>741</v>
+        <v>855</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>43</v>
@@ -4562,7 +4904,7 @@
         <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>742</v>
+        <v>856</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>43</v>
@@ -4676,7 +5018,7 @@
         <v>149</v>
       </c>
       <c r="B21" t="s">
-        <v>743</v>
+        <v>857</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>43</v>
@@ -4737,7 +5079,7 @@
         <v>149</v>
       </c>
       <c r="B22" t="s">
-        <v>744</v>
+        <v>858</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>43</v>
@@ -4798,7 +5140,7 @@
         <v>149</v>
       </c>
       <c r="B23" t="s">
-        <v>745</v>
+        <v>859</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>43</v>
@@ -4912,7 +5254,7 @@
         <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>746</v>
+        <v>860</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>43</v>
@@ -4973,7 +5315,7 @@
         <v>149</v>
       </c>
       <c r="B25" t="s">
-        <v>747</v>
+        <v>861</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>43</v>
@@ -5034,7 +5376,7 @@
         <v>149</v>
       </c>
       <c r="B26" t="s">
-        <v>748</v>
+        <v>862</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>43</v>
@@ -5148,7 +5490,7 @@
         <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>749</v>
+        <v>863</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>43</v>
@@ -5209,7 +5551,7 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>750</v>
+        <v>864</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>43</v>
@@ -5270,7 +5612,7 @@
         <v>149</v>
       </c>
       <c r="B29" t="s">
-        <v>751</v>
+        <v>865</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>43</v>
@@ -5384,7 +5726,7 @@
         <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>752</v>
+        <v>866</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>43</v>
@@ -5445,7 +5787,7 @@
         <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>753</v>
+        <v>867</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>43</v>
@@ -5506,7 +5848,7 @@
         <v>149</v>
       </c>
       <c r="B32" t="s">
-        <v>754</v>
+        <v>868</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>43</v>
@@ -5620,7 +5962,7 @@
         <v>149</v>
       </c>
       <c r="B33" t="s">
-        <v>755</v>
+        <v>869</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>43</v>
@@ -5681,7 +6023,7 @@
         <v>149</v>
       </c>
       <c r="B34" t="s">
-        <v>756</v>
+        <v>870</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>43</v>
@@ -5742,7 +6084,7 @@
         <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>757</v>
+        <v>871</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>43</v>
@@ -5856,7 +6198,7 @@
         <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>758</v>
+        <v>872</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>43</v>
@@ -5917,7 +6259,7 @@
         <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>759</v>
+        <v>873</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>43</v>
@@ -5978,7 +6320,7 @@
         <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>760</v>
+        <v>874</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>43</v>
@@ -6092,7 +6434,7 @@
         <v>149</v>
       </c>
       <c r="B39" t="s">
-        <v>761</v>
+        <v>875</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>43</v>
@@ -6150,10 +6492,10 @@
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B40" t="s">
-        <v>762</v>
+        <v>876</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>43</v>
@@ -6214,7 +6556,7 @@
         <v>149</v>
       </c>
       <c r="B41" t="s">
-        <v>763</v>
+        <v>877</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>43</v>
@@ -6325,10 +6667,10 @@
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" t="s">
-        <v>764</v>
+        <v>878</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>43</v>
@@ -6389,7 +6731,7 @@
         <v>149</v>
       </c>
       <c r="B43" t="s">
-        <v>765</v>
+        <v>879</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>43</v>
@@ -6447,10 +6789,10 @@
     </row>
     <row r="44" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B44" t="s">
-        <v>766</v>
+        <v>880</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>43</v>
@@ -6564,7 +6906,7 @@
         <v>149</v>
       </c>
       <c r="B45" t="s">
-        <v>767</v>
+        <v>881</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>43</v>
@@ -6622,10 +6964,10 @@
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B46" t="s">
-        <v>768</v>
+        <v>882</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>43</v>
@@ -6686,7 +7028,7 @@
         <v>149</v>
       </c>
       <c r="B47" t="s">
-        <v>769</v>
+        <v>883</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>43</v>
@@ -6797,10 +7139,10 @@
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B48" t="s">
-        <v>770</v>
+        <v>884</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>43</v>
@@ -6861,7 +7203,7 @@
         <v>149</v>
       </c>
       <c r="B49" t="s">
-        <v>771</v>
+        <v>885</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>43</v>
@@ -6922,7 +7264,7 @@
         <v>149</v>
       </c>
       <c r="B50" t="s">
-        <v>772</v>
+        <v>886</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>134</v>
@@ -6997,7 +7339,7 @@
         <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>773</v>
+        <v>887</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>134</v>
@@ -7125,7 +7467,7 @@
         <v>149</v>
       </c>
       <c r="B52" t="s">
-        <v>774</v>
+        <v>888</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>134</v>
@@ -7200,7 +7542,7 @@
         <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>775</v>
+        <v>889</v>
       </c>
       <c r="C53" s="1" t="s">
         <v>134</v>
@@ -7328,7 +7670,7 @@
         <v>149</v>
       </c>
       <c r="B54" t="s">
-        <v>776</v>
+        <v>890</v>
       </c>
       <c r="C54" s="1" t="s">
         <v>134</v>
@@ -7403,7 +7745,7 @@
         <v>149</v>
       </c>
       <c r="B55" t="s">
-        <v>777</v>
+        <v>891</v>
       </c>
       <c r="C55" s="1" t="s">
         <v>134</v>
@@ -7531,7 +7873,7 @@
         <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>778</v>
+        <v>892</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>134</v>
@@ -7606,7 +7948,7 @@
         <v>149</v>
       </c>
       <c r="B57" t="s">
-        <v>779</v>
+        <v>893</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>134</v>
@@ -7734,7 +8076,7 @@
         <v>149</v>
       </c>
       <c r="B58" t="s">
-        <v>780</v>
+        <v>894</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>134</v>
@@ -7809,7 +8151,7 @@
         <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>781</v>
+        <v>895</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>134</v>
@@ -7937,7 +8279,7 @@
         <v>149</v>
       </c>
       <c r="B60" t="s">
-        <v>782</v>
+        <v>896</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>134</v>
@@ -8012,7 +8354,7 @@
         <v>149</v>
       </c>
       <c r="B61" t="s">
-        <v>783</v>
+        <v>897</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>134</v>
@@ -8140,7 +8482,7 @@
         <v>150</v>
       </c>
       <c r="B62" t="s">
-        <v>784</v>
+        <v>898</v>
       </c>
       <c r="C62" s="1" t="s">
         <v>134</v>
@@ -8268,7 +8610,7 @@
         <v>149</v>
       </c>
       <c r="B63" t="s">
-        <v>785</v>
+        <v>899</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>134</v>
@@ -8340,10 +8682,10 @@
     </row>
     <row r="64" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B64" t="s">
-        <v>786</v>
+        <v>900</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>134</v>
@@ -8418,7 +8760,7 @@
         <v>149</v>
       </c>
       <c r="B65" t="s">
-        <v>787</v>
+        <v>901</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>134</v>
@@ -8543,10 +8885,10 @@
     </row>
     <row r="66" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B66" t="s">
-        <v>788</v>
+        <v>902</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>134</v>
@@ -8621,7 +8963,7 @@
         <v>149</v>
       </c>
       <c r="B67" t="s">
-        <v>789</v>
+        <v>903</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>134</v>
@@ -8693,10 +9035,10 @@
     </row>
     <row r="68" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B68" t="s">
-        <v>790</v>
+        <v>904</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>134</v>
@@ -8824,7 +9166,7 @@
         <v>149</v>
       </c>
       <c r="B69" t="s">
-        <v>791</v>
+        <v>905</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>134</v>
@@ -8896,10 +9238,10 @@
     </row>
     <row r="70" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B70" t="s">
-        <v>792</v>
+        <v>906</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>134</v>
@@ -8974,7 +9316,7 @@
         <v>149</v>
       </c>
       <c r="B71" t="s">
-        <v>793</v>
+        <v>907</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>134</v>
@@ -9099,10 +9441,10 @@
     </row>
     <row r="72" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B72" t="s">
-        <v>794</v>
+        <v>908</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>134</v>
@@ -9177,7 +9519,7 @@
         <v>149</v>
       </c>
       <c r="B73" t="s">
-        <v>795</v>
+        <v>909</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>134</v>
@@ -9252,7 +9594,7 @@
         <v>149</v>
       </c>
       <c r="B74" t="s">
-        <v>796</v>
+        <v>910</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>135</v>
@@ -9327,7 +9669,7 @@
         <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>797</v>
+        <v>911</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>135</v>
@@ -9455,7 +9797,7 @@
         <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>798</v>
+        <v>912</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>135</v>
@@ -9530,7 +9872,7 @@
         <v>149</v>
       </c>
       <c r="B77" t="s">
-        <v>799</v>
+        <v>913</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>135</v>
@@ -9658,7 +10000,7 @@
         <v>149</v>
       </c>
       <c r="B78" t="s">
-        <v>800</v>
+        <v>914</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>135</v>
@@ -9733,7 +10075,7 @@
         <v>149</v>
       </c>
       <c r="B79" t="s">
-        <v>801</v>
+        <v>915</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>135</v>
@@ -9861,7 +10203,7 @@
         <v>149</v>
       </c>
       <c r="B80" t="s">
-        <v>802</v>
+        <v>916</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>135</v>
@@ -9936,7 +10278,7 @@
         <v>149</v>
       </c>
       <c r="B81" t="s">
-        <v>803</v>
+        <v>917</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>135</v>
@@ -10064,7 +10406,7 @@
         <v>149</v>
       </c>
       <c r="B82" t="s">
-        <v>804</v>
+        <v>918</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>135</v>
@@ -10139,7 +10481,7 @@
         <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>805</v>
+        <v>919</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>135</v>
@@ -10267,7 +10609,7 @@
         <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>806</v>
+        <v>920</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>135</v>
@@ -10342,7 +10684,7 @@
         <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>807</v>
+        <v>921</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>135</v>
@@ -10470,7 +10812,7 @@
         <v>150</v>
       </c>
       <c r="B86" t="s">
-        <v>808</v>
+        <v>922</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>135</v>
@@ -10598,7 +10940,7 @@
         <v>149</v>
       </c>
       <c r="B87" t="s">
-        <v>809</v>
+        <v>923</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>135</v>
@@ -10670,10 +11012,10 @@
     </row>
     <row r="88" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B88" t="s">
-        <v>810</v>
+        <v>924</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>135</v>
@@ -10748,7 +11090,7 @@
         <v>149</v>
       </c>
       <c r="B89" t="s">
-        <v>811</v>
+        <v>925</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>135</v>
@@ -10873,10 +11215,10 @@
     </row>
     <row r="90" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B90" t="s">
-        <v>812</v>
+        <v>926</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>135</v>
@@ -10951,7 +11293,7 @@
         <v>149</v>
       </c>
       <c r="B91" t="s">
-        <v>813</v>
+        <v>927</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>135</v>
@@ -11023,10 +11365,10 @@
     </row>
     <row r="92" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B92" t="s">
-        <v>814</v>
+        <v>928</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>135</v>
@@ -11154,7 +11496,7 @@
         <v>149</v>
       </c>
       <c r="B93" t="s">
-        <v>815</v>
+        <v>929</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>135</v>
@@ -11226,10 +11568,10 @@
     </row>
     <row r="94" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B94" t="s">
-        <v>816</v>
+        <v>930</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>135</v>
@@ -11304,7 +11646,7 @@
         <v>149</v>
       </c>
       <c r="B95" t="s">
-        <v>817</v>
+        <v>931</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>135</v>
@@ -11429,10 +11771,10 @@
     </row>
     <row r="96" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B96" t="s">
-        <v>818</v>
+        <v>932</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>135</v>
@@ -11507,7 +11849,7 @@
         <v>149</v>
       </c>
       <c r="B97" t="s">
-        <v>819</v>
+        <v>933</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>135</v>
@@ -11582,7 +11924,7 @@
         <v>149</v>
       </c>
       <c r="B98" t="s">
-        <v>820</v>
+        <v>934</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>136</v>
@@ -11637,7 +11979,7 @@
         <v>149</v>
       </c>
       <c r="B99" t="s">
-        <v>821</v>
+        <v>935</v>
       </c>
       <c r="C99" s="1" t="s">
         <v>136</v>
@@ -11692,7 +12034,7 @@
         <v>149</v>
       </c>
       <c r="B100" t="s">
-        <v>822</v>
+        <v>936</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>136</v>
@@ -11744,10 +12086,10 @@
     </row>
     <row r="101" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B101" t="s">
-        <v>823</v>
+        <v>937</v>
       </c>
       <c r="C101" s="1" t="s">
         <v>136</v>
@@ -11799,10 +12141,10 @@
     </row>
     <row r="102" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B102" t="s">
-        <v>824</v>
+        <v>938</v>
       </c>
       <c r="C102" s="1" t="s">
         <v>136</v>
@@ -11854,10 +12196,10 @@
     </row>
     <row r="103" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B103" t="s">
-        <v>825</v>
+        <v>939</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>136</v>
@@ -11912,7 +12254,7 @@
         <v>149</v>
       </c>
       <c r="B104" t="s">
-        <v>826</v>
+        <v>940</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>137</v>
@@ -11952,7 +12294,7 @@
         <v>150</v>
       </c>
       <c r="B105" t="s">
-        <v>827</v>
+        <v>941</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>138</v>
@@ -11992,7 +12334,7 @@
         <v>149</v>
       </c>
       <c r="B106" t="s">
-        <v>828</v>
+        <v>942</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>139</v>
@@ -12035,7 +12377,7 @@
         <v>149</v>
       </c>
       <c r="B107" t="s">
-        <v>829</v>
+        <v>943</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>140</v>
@@ -12078,7 +12420,7 @@
         <v>149</v>
       </c>
       <c r="B108" t="s">
-        <v>830</v>
+        <v>944</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>137</v>
@@ -12118,7 +12460,7 @@
         <v>150</v>
       </c>
       <c r="B109" t="s">
-        <v>831</v>
+        <v>945</v>
       </c>
       <c r="C109" s="1" t="s">
         <v>138</v>
@@ -12158,7 +12500,7 @@
         <v>149</v>
       </c>
       <c r="B110" t="s">
-        <v>832</v>
+        <v>946</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>139</v>
@@ -12201,7 +12543,7 @@
         <v>149</v>
       </c>
       <c r="B111" t="s">
-        <v>833</v>
+        <v>947</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>140</v>
@@ -12244,7 +12586,7 @@
         <v>149</v>
       </c>
       <c r="B112" t="s">
-        <v>834</v>
+        <v>948</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>137</v>
@@ -12284,7 +12626,7 @@
         <v>150</v>
       </c>
       <c r="B113" t="s">
-        <v>835</v>
+        <v>949</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>138</v>
@@ -12324,7 +12666,7 @@
         <v>149</v>
       </c>
       <c r="B114" t="s">
-        <v>836</v>
+        <v>950</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>139</v>
@@ -12367,7 +12709,7 @@
         <v>149</v>
       </c>
       <c r="B115" t="s">
-        <v>837</v>
+        <v>951</v>
       </c>
       <c r="C115" s="1" t="s">
         <v>140</v>

</xml_diff>

<commit_message>
Added test data for VSP
</commit_message>
<xml_diff>
--- a/VLinkCCTestData.xlsx
+++ b/VLinkCCTestData.xlsx
@@ -1,28 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\KatalonData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AADF1714-1493-4911-85DE-168F4229A5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{9CE123BF-B458-461F-BD70-52FD68F7AF06}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}"/>
+    <workbookView windowHeight="17640" windowWidth="29040" xWindow="-120" xr2:uid="{8C2F89C9-A10B-4559-913F-0962936A94D9}" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="CCSaleData" sheetId="1" r:id="rId1"/>
-    <sheet name="Trial" sheetId="4" r:id="rId2"/>
-    <sheet name="AuthAndCaptureData" sheetId="3" r:id="rId3"/>
+    <sheet name="CCSaleData" r:id="rId1" sheetId="1"/>
+    <sheet name="Trial" r:id="rId2" sheetId="4"/>
+    <sheet name="AuthAndCaptureData" r:id="rId3" sheetId="3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CCSaleData!$A$1:$A$115</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">CCSaleData!$G$1:$G$115</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6212" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6509" uniqueCount="351">
   <si>
     <t>Notes</t>
   </si>
@@ -839,12 +839,265 @@
   </si>
   <si>
     <t>Mon Apr 04 14:18:08 EDT 2022</t>
+  </si>
+  <si>
+    <t>FDMS</t>
+  </si>
+  <si>
+    <t>COF Initial FDMS</t>
+  </si>
+  <si>
+    <t>COF Subsequent FDMS</t>
+  </si>
+  <si>
+    <t>Req Fields Only FDMS</t>
+  </si>
+  <si>
+    <t>Unencypted track data FDMS</t>
+  </si>
+  <si>
+    <t>Unencypted track1 data FDMS</t>
+  </si>
+  <si>
+    <t>Unencypted track2 data FDMS</t>
+  </si>
+  <si>
+    <t>Unencypted track1 And 2 data FDMS</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:20:05 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:20:55 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:21:42 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:22:29 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:23:16 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:24:02 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:24:49 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:25:36 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:26:22 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:27:08 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:27:55 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:28:42 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:29:28 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:30:14 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:31:00 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:31:46 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:32:32 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:33:18 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:34:05 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:34:50 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:35:35 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:36:22 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:37:08 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:37:54 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:38:41 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:39:26 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:40:12 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:40:59 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:41:45 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:42:31 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:43:17 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:44:04 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:44:50 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:45:39 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:46:25 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:47:11 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:47:58 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:48:44 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:49:31 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:50:17 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:51:03 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:51:48 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:52:35 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:53:21 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:54:07 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:54:52 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:55:38 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:56:24 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:57:11 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:57:57 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:58:43 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 12:59:28 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:00:15 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:00:59 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:01:46 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:02:32 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:03:18 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:04:03 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:04:49 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:05:35 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:06:22 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:07:09 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:07:55 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:08:41 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:09:28 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:10:12 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:10:57 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:11:44 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:12:30 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:13:14 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:14:01 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:14:47 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:15:34 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:16:18 EDT 2022</t>
+  </si>
+  <si>
+    <t>Mon Apr 18 13:17:04 EDT 2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -893,20 +1146,20 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -923,10 +1176,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -961,7 +1214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1013,7 +1266,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1124,21 +1377,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1155,7 +1408,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1207,81 +1460,82 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}">
-  <dimension ref="A1:AX115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}">
+  <dimension ref="A1:AY115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D115"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A59" ySplit="1"/>
+      <selection activeCell="A115" pane="bottomLeft" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" collapsed="1"/>
-    <col min="3" max="4" width="32" style="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="4.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="5.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="24" style="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="4.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="8.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="115.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="75.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="40.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="14.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="13.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="45" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="46" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="47" max="48" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="12.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="14.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="11.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="15.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="15.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="11.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="18.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="60" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="61" max="62" width="15.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="16.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="65" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="66" max="16384" width="26.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="36.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" style="1" width="32.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="4.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="5.5703125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="24.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="4.7109375" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="8.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="115.42578125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="75.5703125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="40.5703125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="13.5703125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="37" max="45" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="46" max="46" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="47" max="48" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" style="1" width="12.5703125" collapsed="true"/>
+    <col min="50" max="50" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
+    <col min="60" max="60" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="61" max="62" bestFit="true" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="65" max="65" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="66" max="16384" style="1" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
@@ -1435,10 +1689,13 @@
     </row>
     <row r="2" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B2" t="s">
-        <v>266</v>
+        <v>276</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>259</v>
@@ -1555,7 +1812,10 @@
         <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>277</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>259</v>
@@ -1619,7 +1879,10 @@
         <v>149</v>
       </c>
       <c r="B4" t="s">
-        <v>152</v>
+        <v>278</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>259</v>
@@ -1683,7 +1946,10 @@
         <v>149</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>279</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>259</v>
@@ -1800,7 +2066,10 @@
         <v>149</v>
       </c>
       <c r="B6" t="s">
-        <v>154</v>
+        <v>280</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>259</v>
@@ -1864,7 +2133,10 @@
         <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>281</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>259</v>
@@ -1928,7 +2200,10 @@
         <v>149</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>282</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>259</v>
@@ -2045,7 +2320,10 @@
         <v>149</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>283</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>259</v>
@@ -2109,7 +2387,10 @@
         <v>149</v>
       </c>
       <c r="B10" t="s">
-        <v>158</v>
+        <v>284</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>259</v>
@@ -2173,7 +2454,10 @@
         <v>149</v>
       </c>
       <c r="B11" t="s">
-        <v>159</v>
+        <v>285</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>259</v>
@@ -2290,7 +2574,10 @@
         <v>149</v>
       </c>
       <c r="B12" t="s">
-        <v>160</v>
+        <v>286</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>259</v>
@@ -2354,7 +2641,10 @@
         <v>149</v>
       </c>
       <c r="B13" t="s">
-        <v>161</v>
+        <v>287</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>259</v>
@@ -2418,7 +2708,10 @@
         <v>149</v>
       </c>
       <c r="B14" t="s">
-        <v>162</v>
+        <v>288</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>259</v>
@@ -2535,7 +2828,10 @@
         <v>149</v>
       </c>
       <c r="B15" t="s">
-        <v>163</v>
+        <v>289</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>259</v>
@@ -2599,7 +2895,10 @@
         <v>149</v>
       </c>
       <c r="B16" t="s">
-        <v>164</v>
+        <v>290</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>259</v>
@@ -2663,7 +2962,10 @@
         <v>149</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>291</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>259</v>
@@ -2780,7 +3082,10 @@
         <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>166</v>
+        <v>292</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>259</v>
@@ -2844,7 +3149,10 @@
         <v>149</v>
       </c>
       <c r="B19" t="s">
-        <v>167</v>
+        <v>293</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>259</v>
@@ -2908,7 +3216,10 @@
         <v>149</v>
       </c>
       <c r="B20" t="s">
-        <v>168</v>
+        <v>294</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>259</v>
@@ -3025,7 +3336,10 @@
         <v>149</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>295</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>259</v>
@@ -3089,7 +3403,10 @@
         <v>149</v>
       </c>
       <c r="B22" t="s">
-        <v>170</v>
+        <v>296</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>259</v>
@@ -3153,7 +3470,10 @@
         <v>149</v>
       </c>
       <c r="B23" t="s">
-        <v>171</v>
+        <v>297</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>259</v>
@@ -3270,7 +3590,10 @@
         <v>149</v>
       </c>
       <c r="B24" t="s">
-        <v>172</v>
+        <v>298</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>259</v>
@@ -3334,7 +3657,10 @@
         <v>149</v>
       </c>
       <c r="B25" t="s">
-        <v>173</v>
+        <v>299</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>259</v>
@@ -3395,10 +3721,13 @@
     </row>
     <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B26" t="s">
-        <v>174</v>
+        <v>300</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>259</v>
@@ -3515,7 +3844,10 @@
         <v>149</v>
       </c>
       <c r="B27" t="s">
-        <v>175</v>
+        <v>301</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>259</v>
@@ -3579,7 +3911,10 @@
         <v>149</v>
       </c>
       <c r="B28" t="s">
-        <v>176</v>
+        <v>302</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>259</v>
@@ -3643,7 +3978,10 @@
         <v>149</v>
       </c>
       <c r="B29" t="s">
-        <v>177</v>
+        <v>303</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>259</v>
@@ -3760,7 +4098,10 @@
         <v>149</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>304</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>259</v>
@@ -3824,7 +4165,10 @@
         <v>149</v>
       </c>
       <c r="B31" t="s">
-        <v>179</v>
+        <v>305</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>259</v>
@@ -3888,7 +4232,10 @@
         <v>149</v>
       </c>
       <c r="B32" t="s">
-        <v>180</v>
+        <v>306</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>259</v>
@@ -4005,7 +4352,10 @@
         <v>149</v>
       </c>
       <c r="B33" t="s">
-        <v>181</v>
+        <v>307</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>259</v>
@@ -4069,7 +4419,10 @@
         <v>149</v>
       </c>
       <c r="B34" t="s">
-        <v>182</v>
+        <v>308</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>259</v>
@@ -4133,7 +4486,10 @@
         <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>183</v>
+        <v>309</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>259</v>
@@ -4250,7 +4606,10 @@
         <v>149</v>
       </c>
       <c r="B36" t="s">
-        <v>184</v>
+        <v>310</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>259</v>
@@ -4314,7 +4673,10 @@
         <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>185</v>
+        <v>311</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>267</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>259</v>
@@ -4380,9 +4742,6 @@
       <c r="B38" t="s">
         <v>260</v>
       </c>
-      <c r="D38" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E38" s="1" t="s">
         <v>43</v>
       </c>
@@ -4497,9 +4856,6 @@
       <c r="B39" t="s">
         <v>186</v>
       </c>
-      <c r="D39" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E39" s="1" t="s">
         <v>43</v>
       </c>
@@ -4561,9 +4917,6 @@
       <c r="B40" t="s">
         <v>187</v>
       </c>
-      <c r="D40" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E40" s="1" t="s">
         <v>43</v>
       </c>
@@ -4625,9 +4978,6 @@
       <c r="B41" t="s">
         <v>188</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E41" s="1" t="s">
         <v>43</v>
       </c>
@@ -4742,9 +5092,6 @@
       <c r="B42" t="s">
         <v>189</v>
       </c>
-      <c r="D42" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E42" s="1" t="s">
         <v>43</v>
       </c>
@@ -4806,9 +5153,6 @@
       <c r="B43" t="s">
         <v>190</v>
       </c>
-      <c r="D43" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E43" s="1" t="s">
         <v>43</v>
       </c>
@@ -4870,9 +5214,6 @@
       <c r="B44" t="s">
         <v>191</v>
       </c>
-      <c r="D44" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E44" s="1" t="s">
         <v>43</v>
       </c>
@@ -4987,9 +5328,6 @@
       <c r="B45" t="s">
         <v>192</v>
       </c>
-      <c r="D45" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E45" s="1" t="s">
         <v>43</v>
       </c>
@@ -5051,9 +5389,6 @@
       <c r="B46" t="s">
         <v>193</v>
       </c>
-      <c r="D46" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E46" s="1" t="s">
         <v>43</v>
       </c>
@@ -5115,9 +5450,6 @@
       <c r="B47" t="s">
         <v>194</v>
       </c>
-      <c r="D47" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E47" s="1" t="s">
         <v>43</v>
       </c>
@@ -5232,9 +5564,6 @@
       <c r="B48" t="s">
         <v>195</v>
       </c>
-      <c r="D48" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E48" s="1" t="s">
         <v>43</v>
       </c>
@@ -5296,9 +5625,6 @@
       <c r="B49" t="s">
         <v>196</v>
       </c>
-      <c r="D49" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E49" s="1" t="s">
         <v>43</v>
       </c>
@@ -5358,10 +5684,10 @@
         <v>149</v>
       </c>
       <c r="B50" t="s">
-        <v>197</v>
+        <v>312</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>259</v>
@@ -5436,10 +5762,10 @@
         <v>149</v>
       </c>
       <c r="B51" t="s">
-        <v>198</v>
+        <v>313</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>259</v>
@@ -5567,10 +5893,10 @@
         <v>149</v>
       </c>
       <c r="B52" t="s">
-        <v>199</v>
+        <v>314</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>259</v>
@@ -5645,10 +5971,10 @@
         <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>200</v>
+        <v>315</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>259</v>
@@ -5773,13 +6099,13 @@
     </row>
     <row r="54" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>201</v>
+        <v>316</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>259</v>
@@ -5854,10 +6180,10 @@
         <v>149</v>
       </c>
       <c r="B55" t="s">
-        <v>202</v>
+        <v>317</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>259</v>
@@ -5985,10 +6311,10 @@
         <v>149</v>
       </c>
       <c r="B56" t="s">
-        <v>203</v>
+        <v>318</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>259</v>
@@ -6063,10 +6389,10 @@
         <v>149</v>
       </c>
       <c r="B57" t="s">
-        <v>204</v>
+        <v>319</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>259</v>
@@ -6191,13 +6517,13 @@
     </row>
     <row r="58" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B58" t="s">
-        <v>205</v>
+        <v>320</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>259</v>
@@ -6272,10 +6598,10 @@
         <v>149</v>
       </c>
       <c r="B59" t="s">
-        <v>206</v>
+        <v>321</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>259</v>
@@ -6403,10 +6729,10 @@
         <v>149</v>
       </c>
       <c r="B60" t="s">
-        <v>207</v>
+        <v>322</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>259</v>
@@ -6481,10 +6807,10 @@
         <v>149</v>
       </c>
       <c r="B61" t="s">
-        <v>208</v>
+        <v>323</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>134</v>
+        <v>268</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>259</v>
@@ -6617,9 +6943,6 @@
       <c r="C62" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E62" s="1" t="s">
         <v>43</v>
       </c>
@@ -6748,9 +7071,6 @@
       <c r="C63" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E63" s="1" t="s">
         <v>43</v>
       </c>
@@ -6826,9 +7146,6 @@
       <c r="C64" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E64" s="1" t="s">
         <v>43</v>
       </c>
@@ -6904,9 +7221,6 @@
       <c r="C65" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D65" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E65" s="1" t="s">
         <v>43</v>
       </c>
@@ -7035,9 +7349,6 @@
       <c r="C66" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D66" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E66" s="1" t="s">
         <v>43</v>
       </c>
@@ -7113,9 +7424,6 @@
       <c r="C67" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D67" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E67" s="1" t="s">
         <v>43</v>
       </c>
@@ -7191,9 +7499,6 @@
       <c r="C68" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E68" s="1" t="s">
         <v>43</v>
       </c>
@@ -7322,9 +7627,6 @@
       <c r="C69" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D69" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E69" s="1" t="s">
         <v>43</v>
       </c>
@@ -7400,9 +7702,6 @@
       <c r="C70" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D70" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E70" s="1" t="s">
         <v>43</v>
       </c>
@@ -7478,9 +7777,6 @@
       <c r="C71" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D71" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E71" s="1" t="s">
         <v>43</v>
       </c>
@@ -7609,9 +7905,6 @@
       <c r="C72" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D72" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E72" s="1" t="s">
         <v>43</v>
       </c>
@@ -7687,9 +7980,6 @@
       <c r="C73" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D73" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E73" s="1" t="s">
         <v>43</v>
       </c>
@@ -7760,10 +8050,10 @@
         <v>149</v>
       </c>
       <c r="B74" t="s">
-        <v>220</v>
+        <v>324</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>259</v>
@@ -7838,10 +8128,10 @@
         <v>149</v>
       </c>
       <c r="B75" t="s">
-        <v>221</v>
+        <v>325</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>259</v>
@@ -7969,10 +8259,10 @@
         <v>149</v>
       </c>
       <c r="B76" t="s">
-        <v>222</v>
+        <v>326</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>259</v>
@@ -8047,10 +8337,10 @@
         <v>149</v>
       </c>
       <c r="B77" t="s">
-        <v>223</v>
+        <v>327</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>259</v>
@@ -8175,13 +8465,13 @@
     </row>
     <row r="78" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B78" t="s">
-        <v>224</v>
+        <v>328</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>259</v>
@@ -8256,10 +8546,10 @@
         <v>149</v>
       </c>
       <c r="B79" t="s">
-        <v>225</v>
+        <v>329</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>259</v>
@@ -8387,10 +8677,10 @@
         <v>149</v>
       </c>
       <c r="B80" t="s">
-        <v>226</v>
+        <v>330</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>259</v>
@@ -8465,10 +8755,10 @@
         <v>149</v>
       </c>
       <c r="B81" t="s">
-        <v>227</v>
+        <v>331</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>259</v>
@@ -8593,13 +8883,13 @@
     </row>
     <row r="82" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B82" t="s">
-        <v>228</v>
+        <v>332</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>259</v>
@@ -8674,10 +8964,10 @@
         <v>149</v>
       </c>
       <c r="B83" t="s">
-        <v>229</v>
+        <v>333</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>259</v>
@@ -8805,10 +9095,10 @@
         <v>149</v>
       </c>
       <c r="B84" t="s">
-        <v>230</v>
+        <v>334</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D84" s="1" t="s">
         <v>259</v>
@@ -8883,10 +9173,10 @@
         <v>149</v>
       </c>
       <c r="B85" t="s">
-        <v>231</v>
+        <v>335</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>135</v>
+        <v>269</v>
       </c>
       <c r="D85" s="1" t="s">
         <v>259</v>
@@ -9019,9 +9309,6 @@
       <c r="C86" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D86" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E86" s="1" t="s">
         <v>43</v>
       </c>
@@ -9150,9 +9437,6 @@
       <c r="C87" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D87" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E87" s="1" t="s">
         <v>43</v>
       </c>
@@ -9228,9 +9512,6 @@
       <c r="C88" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D88" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E88" s="1" t="s">
         <v>43</v>
       </c>
@@ -9306,9 +9587,6 @@
       <c r="C89" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D89" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E89" s="1" t="s">
         <v>43</v>
       </c>
@@ -9437,9 +9715,6 @@
       <c r="C90" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D90" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E90" s="1" t="s">
         <v>43</v>
       </c>
@@ -9515,9 +9790,6 @@
       <c r="C91" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D91" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E91" s="1" t="s">
         <v>43</v>
       </c>
@@ -9593,9 +9865,6 @@
       <c r="C92" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D92" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E92" s="1" t="s">
         <v>43</v>
       </c>
@@ -9724,9 +9993,6 @@
       <c r="C93" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D93" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E93" s="1" t="s">
         <v>43</v>
       </c>
@@ -9802,9 +10068,6 @@
       <c r="C94" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D94" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E94" s="1" t="s">
         <v>43</v>
       </c>
@@ -9880,9 +10143,6 @@
       <c r="C95" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D95" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E95" s="1" t="s">
         <v>43</v>
       </c>
@@ -10011,9 +10271,6 @@
       <c r="C96" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D96" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E96" s="1" t="s">
         <v>43</v>
       </c>
@@ -10089,9 +10346,6 @@
       <c r="C97" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="D97" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E97" s="1" t="s">
         <v>43</v>
       </c>
@@ -10159,13 +10413,13 @@
     </row>
     <row r="98" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B98" t="s">
-        <v>243</v>
+        <v>336</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>136</v>
+        <v>270</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>259</v>
@@ -10220,10 +10474,10 @@
         <v>149</v>
       </c>
       <c r="B99" t="s">
-        <v>244</v>
+        <v>337</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>136</v>
+        <v>270</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>259</v>
@@ -10278,10 +10532,10 @@
         <v>149</v>
       </c>
       <c r="B100" t="s">
-        <v>245</v>
+        <v>338</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>136</v>
+        <v>270</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>259</v>
@@ -10341,9 +10595,6 @@
       <c r="C101" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D101" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E101" s="1" t="s">
         <v>43</v>
       </c>
@@ -10399,9 +10650,6 @@
       <c r="C102" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D102" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E102" s="1" t="s">
         <v>43</v>
       </c>
@@ -10457,9 +10705,6 @@
       <c r="C103" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="D103" s="1" t="s">
-        <v>259</v>
-      </c>
       <c r="E103" s="1" t="s">
         <v>43</v>
       </c>
@@ -10510,10 +10755,10 @@
         <v>149</v>
       </c>
       <c r="B104" t="s">
-        <v>249</v>
+        <v>339</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>137</v>
+        <v>271</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>259</v>
@@ -10553,10 +10798,10 @@
         <v>150</v>
       </c>
       <c r="B105" t="s">
-        <v>263</v>
+        <v>340</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>138</v>
+        <v>272</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>259</v>
@@ -10596,10 +10841,10 @@
         <v>149</v>
       </c>
       <c r="B106" t="s">
-        <v>250</v>
+        <v>341</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>139</v>
+        <v>273</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>259</v>
@@ -10642,10 +10887,10 @@
         <v>149</v>
       </c>
       <c r="B107" t="s">
-        <v>251</v>
+        <v>342</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>140</v>
+        <v>274</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>259</v>
@@ -10688,10 +10933,10 @@
         <v>149</v>
       </c>
       <c r="B108" t="s">
-        <v>252</v>
+        <v>343</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>137</v>
+        <v>271</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>259</v>
@@ -10731,10 +10976,10 @@
         <v>150</v>
       </c>
       <c r="B109" t="s">
-        <v>264</v>
+        <v>344</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>138</v>
+        <v>272</v>
       </c>
       <c r="D109" s="1" t="s">
         <v>259</v>
@@ -10774,10 +11019,10 @@
         <v>149</v>
       </c>
       <c r="B110" t="s">
-        <v>253</v>
+        <v>345</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>139</v>
+        <v>273</v>
       </c>
       <c r="D110" s="1" t="s">
         <v>259</v>
@@ -10820,10 +11065,10 @@
         <v>149</v>
       </c>
       <c r="B111" t="s">
-        <v>254</v>
+        <v>346</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>140</v>
+        <v>274</v>
       </c>
       <c r="D111" s="1" t="s">
         <v>259</v>
@@ -10866,10 +11111,10 @@
         <v>149</v>
       </c>
       <c r="B112" t="s">
-        <v>255</v>
+        <v>347</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>137</v>
+        <v>271</v>
       </c>
       <c r="D112" s="1" t="s">
         <v>259</v>
@@ -10909,10 +11154,10 @@
         <v>150</v>
       </c>
       <c r="B113" t="s">
-        <v>265</v>
+        <v>348</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>138</v>
+        <v>272</v>
       </c>
       <c r="D113" s="1" t="s">
         <v>259</v>
@@ -10952,10 +11197,10 @@
         <v>149</v>
       </c>
       <c r="B114" t="s">
-        <v>256</v>
+        <v>349</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>139</v>
+        <v>273</v>
       </c>
       <c r="D114" s="1" t="s">
         <v>259</v>
@@ -10998,10 +11243,10 @@
         <v>149</v>
       </c>
       <c r="B115" t="s">
-        <v>257</v>
+        <v>350</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>140</v>
+        <v>274</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>259</v>
@@ -11040,16 +11285,16 @@
       <c r="AX115" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A115" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}"/>
+  <autoFilter ref="G1:G115" xr:uid="{01D907F6-7637-41F5-9F0A-BDDAA86240AA}"/>
   <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E373AFE3-95E6-4012-963C-FB304E9ADB66}">
-  <dimension ref="A1:AW115"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E373AFE3-95E6-4012-963C-FB304E9ADB66}">
+  <dimension ref="A1:AX115"/>
   <sheetViews>
     <sheetView topLeftCell="A106" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
@@ -11057,64 +11302,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="26.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="26.7109375" style="1" collapsed="1"/>
-    <col min="3" max="3" width="32" style="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="4.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="6.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="9.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="11.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="8.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="6.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="19.140625" style="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="22.28515625" style="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="8" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="5.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="6" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="9.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="24" style="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="4.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.85546875" style="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="8.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="9.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="115.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="75.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="40.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="14.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="23.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="13.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="11.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="18" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="7" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="44" width="10.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="45" max="45" width="11.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="46" max="47" width="13.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="48" max="48" width="12.5703125" style="1" customWidth="1" collapsed="1"/>
-    <col min="49" max="49" width="15" style="1" customWidth="1" collapsed="1"/>
-    <col min="50" max="50" width="14.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="9.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="52" max="52" width="12" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="53" max="53" width="11.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="15.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="55" max="55" width="14.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="56" max="56" width="15.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="57" max="57" width="11.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="58" max="58" width="18.28515625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="59" max="59" width="14.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="60" max="61" width="15.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="62" max="62" width="16.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="63" max="63" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="64" max="64" width="10.7109375" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="65" max="16384" width="26.7109375" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="2" max="2" style="1" width="26.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="32.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="4.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="9.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" style="1" width="11.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="1" width="6.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" style="1" width="19.140625" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="1" width="22.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="8.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="5.5703125" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="9.85546875" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="8.140625" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" style="1" width="24.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="4.7109375" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="8.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="9.28515625" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="115.42578125" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="75.5703125" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="40.5703125" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="1" width="23.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="1" width="13.5703125" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="1" width="11.140625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" style="1" width="18.0" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="1" width="7.0" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="36" max="44" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" style="1" width="11.42578125" collapsed="true"/>
+    <col min="46" max="47" bestFit="true" customWidth="true" style="1" width="13.7109375" collapsed="true"/>
+    <col min="48" max="48" customWidth="true" style="1" width="12.5703125" collapsed="true"/>
+    <col min="49" max="49" customWidth="true" style="1" width="15.0" collapsed="true"/>
+    <col min="50" max="50" bestFit="true" customWidth="true" style="1" width="14.42578125" collapsed="true"/>
+    <col min="51" max="51" bestFit="true" customWidth="true" style="1" width="9.140625" collapsed="true"/>
+    <col min="52" max="52" bestFit="true" customWidth="true" style="1" width="12.0" collapsed="true"/>
+    <col min="53" max="53" bestFit="true" customWidth="true" style="1" width="11.5703125" collapsed="true"/>
+    <col min="54" max="54" bestFit="true" customWidth="true" style="1" width="15.28515625" collapsed="true"/>
+    <col min="55" max="55" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="56" max="56" bestFit="true" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="57" max="57" bestFit="true" customWidth="true" style="1" width="11.85546875" collapsed="true"/>
+    <col min="58" max="58" bestFit="true" customWidth="true" style="1" width="18.28515625" collapsed="true"/>
+    <col min="59" max="59" bestFit="true" customWidth="true" style="1" width="14.85546875" collapsed="true"/>
+    <col min="60" max="61" bestFit="true" customWidth="true" style="1" width="15.85546875" collapsed="true"/>
+    <col min="62" max="62" bestFit="true" customWidth="true" style="1" width="16.42578125" collapsed="true"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="64" max="64" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="65" max="16384" style="1" width="26.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:49" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
@@ -20528,13 +20773,13 @@
       <c r="AW115" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E51003-E6AF-4A46-8DE2-C02177084CDE}">
-  <dimension ref="A1:BS1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97E51003-E6AF-4A46-8DE2-C02177084CDE}">
+  <dimension ref="A1:BT1"/>
   <sheetViews>
     <sheetView topLeftCell="BC1" workbookViewId="0">
       <selection activeCell="BE29" sqref="BE29"/>
@@ -20542,10 +20787,10 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="20.42578125" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="20.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -20761,7 +21006,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="4294967293" orientation="portrait" r:id="rId1" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>